<commit_message>
update empty to contain a table for data
</commit_message>
<xml_diff>
--- a/static/ledger-empty.xlsx
+++ b/static/ledger-empty.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6DE48E0-3F5D-406E-BBC9-333F598FD06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8463E10-A895-40D9-A15A-B1FC3A709AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,6 +23,50 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Date/Time</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Subcode</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>Buy/Sell</t>
+  </si>
+  <si>
+    <t>Open/Close</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Fees</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -73,6 +117,27 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{424936DA-4101-48B5-B1BE-9A7B5EA9F6B7}" name="Table1" displayName="Table1" ref="A4:L688" totalsRowShown="0">
+  <autoFilter ref="A4:L688" xr:uid="{424936DA-4101-48B5-B1BE-9A7B5EA9F6B7}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{D3CA2164-4FEF-4CFF-8489-11AE4F9407AA}" name="Date/Time"/>
+    <tableColumn id="2" xr3:uid="{F3248CF6-9349-4191-9B5E-DF70DC19D196}" name="Code"/>
+    <tableColumn id="3" xr3:uid="{AC9015B4-D595-4697-928A-6EE25015BBFD}" name="Subcode"/>
+    <tableColumn id="4" xr3:uid="{0E6431CF-391F-48D6-9FC6-B1859D90A048}" name="Symbol"/>
+    <tableColumn id="5" xr3:uid="{232E1253-054B-4771-B21A-030865C59220}" name="Buy/Sell"/>
+    <tableColumn id="6" xr3:uid="{FBFE3094-2DFA-4843-A939-F248FC1F8C58}" name="Open/Close"/>
+    <tableColumn id="7" xr3:uid="{C96C4C1E-B1AF-4447-B8AC-1FCAFD5D4A70}" name="Quantity"/>
+    <tableColumn id="8" xr3:uid="{D34D13E3-3EF6-4518-903A-6D2730305EF4}" name="Price"/>
+    <tableColumn id="9" xr3:uid="{C844FA26-CD5A-4578-ACFB-49A6C67212DE}" name="Fees"/>
+    <tableColumn id="10" xr3:uid="{7E4B95B2-E855-420C-9421-7334A482DD61}" name="Amount"/>
+    <tableColumn id="11" xr3:uid="{1D32F471-AB70-4B4D-A025-BFAACCD5A95E}" name="Description"/>
+    <tableColumn id="12" xr3:uid="{C36BB8C1-D4AA-47D2-96B9-64445E38C3E5}" name="Account"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -372,12 +437,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A4:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>